<commit_message>
location.xlsx can add other column
</commit_message>
<xml_diff>
--- a/sample/locationtest/output/custom/location.xlsx
+++ b/sample/locationtest/output/custom/location.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>id</t>
   </si>
@@ -38,9 +38,15 @@
     <t>en</t>
   </si>
   <si>
+    <t>备注</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
+    <t>空字符串</t>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
@@ -50,6 +56,9 @@
     <t>Apple</t>
   </si>
   <si>
+    <t>备注1</t>
+  </si>
+  <si>
     <t>3</t>
   </si>
   <si>
@@ -59,6 +68,12 @@
     <t>Bnana</t>
   </si>
   <si>
+    <t>备注2</t>
+  </si>
+  <si>
+    <t>是非得失</t>
+  </si>
+  <si>
     <t>4</t>
   </si>
   <si>
@@ -68,6 +83,9 @@
     <t>peal</t>
   </si>
   <si>
+    <t>备注3</t>
+  </si>
+  <si>
     <t>5</t>
   </si>
   <si>
@@ -77,16 +95,25 @@
     <t>middle</t>
   </si>
   <si>
+    <t>备注4</t>
+  </si>
+  <si>
     <t>6</t>
   </si>
   <si>
     <t>中秋节礼包</t>
   </si>
   <si>
+    <t>备注5</t>
+  </si>
+  <si>
     <t>7</t>
   </si>
   <si>
     <t>中秋节鞋子</t>
+  </si>
+  <si>
+    <t>备注6</t>
   </si>
 </sst>
 </file>
@@ -561,7 +588,7 @@
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1246,18 +1273,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="7" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="7" outlineLevelCol="7"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1267,70 +1294,97 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>